<commit_message>
Added first page index.html
</commit_message>
<xml_diff>
--- a/jalon 1/Gestion du temps.xlsx
+++ b/jalon 1/Gestion du temps.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cda5pani\OneDrive - AMIO\Fil Rouge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cda5pani\OneDrive - AMIO\Fil Rouge\jalon 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Jalon 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Jalon 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>demi-journée</t>
   </si>
@@ -159,6 +160,24 @@
   </si>
   <si>
     <t>temps passé</t>
+  </si>
+  <si>
+    <t>prise de connaissance du fil rouge</t>
+  </si>
+  <si>
+    <t>Rédaction de la maquette, ranger dossier et MAJ Git</t>
+  </si>
+  <si>
+    <t>Maquette</t>
+  </si>
+  <si>
+    <t>temps passé (en heures)</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>Rédaction de la maquette, début html</t>
   </si>
 </sst>
 </file>
@@ -572,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,4 +1091,153 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="43.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <f>F2-D2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G12" si="0">F3-D3</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Gestion du temps
</commit_message>
<xml_diff>
--- a/jalon 1/Gestion du temps.xlsx
+++ b/jalon 1/Gestion du temps.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>demi-journée</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>CSS header, fond d'écran</t>
+  </si>
+  <si>
+    <t>CSS responsive, SASS</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1119,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,7 +1209,7 @@
         <v>54</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -1216,7 +1219,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1230,7 +1233,7 @@
         <v>55</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1240,7 +1243,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1280,6 +1283,12 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
       <c r="G9">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
Unified header footer to all visitor pages html css js
</commit_message>
<xml_diff>
--- a/jalon 1/Gestion du temps.xlsx
+++ b/jalon 1/Gestion du temps.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>demi-journée</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>CSS responsive, SASS</t>
+  </si>
+  <si>
+    <t>git</t>
+  </si>
+  <si>
+    <t>Non applicable</t>
+  </si>
+  <si>
+    <t>non applicable</t>
+  </si>
+  <si>
+    <t>SCSS, CSS, appliquer le template.css à toutes les pages</t>
   </si>
 </sst>
 </file>
@@ -1119,12 +1131,14 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.44140625" customWidth="1"/>
+    <col min="2" max="2" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
@@ -1185,7 +1199,7 @@
         <v>49</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -1195,7 +1209,7 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G12" si="0">F3-D3</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1209,7 +1223,7 @@
         <v>54</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -1219,7 +1233,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1253,9 +1267,20 @@
       <c r="B6" t="s">
         <v>52</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1295,12 +1320,24 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
       <c r="G10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
       <c r="G11">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
Saved from Nouveau Fil Rouge
</commit_message>
<xml_diff>
--- a/jalon 1/Gestion du temps.xlsx
+++ b/jalon 1/Gestion du temps.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>demi-journée</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>menu responsive</t>
+  </si>
+  <si>
+    <t>Galerie responsive sur page d'accueil</t>
   </si>
 </sst>
 </file>
@@ -1131,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1202,7 +1205,7 @@
         <v>49</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -1212,7 +1215,7 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G12" si="0">F3-D3</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1226,7 +1229,7 @@
         <v>54</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -1236,7 +1239,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1250,7 +1253,7 @@
         <v>55</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1260,7 +1263,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1364,6 +1367,38 @@
       </c>
       <c r="B13" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>